<commit_message>
Add Planning xls to support README file
</commit_message>
<xml_diff>
--- a/readme-docs/TCC_Planning.xlsx
+++ b/readme-docs/TCC_Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrric\Documents\Rick\Coding\Project 5_The Coffee Collective\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8208F16F-488C-4F90-863E-8616A4FD4C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE5EC57-F712-4043-9D11-F31F0CA06589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="-17490" windowWidth="29040" windowHeight="15720" xr2:uid="{A5890AFF-ADB8-40C3-9B84-BBA54327EE61}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{A5890AFF-ADB8-40C3-9B84-BBA54327EE61}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Thinking" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="539">
   <si>
     <t>Empathize (knowing the users) and Defining (the what)</t>
   </si>
@@ -1747,14 +1747,6 @@
     <t>fields/image_url</t>
   </si>
   <si>
-    <t>a. Header with branding encompassed as part of the NavBar
-b. Option to explore site through main menu links; Useful Links, About Us, Contact Us, Accessibility Statement, User Agreement, Copyright Info
-c. Quick link to search products in Navbar
-d. Navbar will be fixed to support user navigation
-e. User account function added to Navbar
-f. NavBar will change in layout for mobile devices with collapsed menus</t>
-  </si>
-  <si>
     <t xml:space="preserve">a. Create a section on the homepage that highlights business location and opening times, including a Google Map
 </t>
   </si>
@@ -1821,6 +1813,44 @@
   </si>
   <si>
     <t>Link to the register for the newsletter will be within a section of the homepage</t>
+  </si>
+  <si>
+    <t>F40</t>
+  </si>
+  <si>
+    <t>US38</t>
+  </si>
+  <si>
+    <t>Registered users can save items they wish to purchase to a list for a later date</t>
+  </si>
+  <si>
+    <t>Wish list</t>
+  </si>
+  <si>
+    <t>As a registered user/member, I can save products I may wish to buy, so that I can come back and see a short-list when I'm ready to purchase</t>
+  </si>
+  <si>
+    <t>a. Header with branding encompassed as part of the Navbar
+b. Option to explore site through main menu links; Useful Links, About Us, Contact Us, Accessibility Statement, User Agreement, Copyright Info
+c. Quick link to search products in Navbar
+d. Navbar will be fixed to support user navigation
+e. User account function added to Navbar
+f. Navbar will change in layout for mobile devices with collapsed menus</t>
+  </si>
+  <si>
+    <t>1. Signed-in users have access to using an optional wish list
+2. Signed-in users can add items to their wish list from the product page and remove from the wish list page
+3. The wish list feature is not available to non members</t>
+  </si>
+  <si>
+    <t>a. Create the model , views and url for the Wish List
+b. Create a html page for the Wish List
+c. Add relevant links to the Wish List page
+d. Create buttons and functionality to add items to the Wish List from the products page
+e. Create button in Wish List page to remove items from the Wish List</t>
+  </si>
+  <si>
+    <t>Wish List</t>
   </si>
 </sst>
 </file>
@@ -2086,7 +2116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2198,15 +2228,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2264,9 +2285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2277,11 +2295,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2585,13 +2612,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92EC34CB-BD79-4B37-B8C2-29C2438B4EF8}" name="Table3" displayName="Table3" ref="A1:G40" totalsRowShown="0" dataDxfId="20">
-  <autoFilter ref="A1:G40" xr:uid="{92EC34CB-BD79-4B37-B8C2-29C2438B4EF8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
-    <sortCondition ref="D2:D40"/>
-    <sortCondition ref="E2:E40"/>
-    <sortCondition ref="F2:F40"/>
-    <sortCondition ref="G2:G40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92EC34CB-BD79-4B37-B8C2-29C2438B4EF8}" name="Table3" displayName="Table3" ref="A1:G41" totalsRowShown="0" dataDxfId="20">
+  <autoFilter ref="A1:G41" xr:uid="{92EC34CB-BD79-4B37-B8C2-29C2438B4EF8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G41">
+    <sortCondition ref="D2:D41"/>
+    <sortCondition ref="E2:E41"/>
+    <sortCondition ref="F2:F41"/>
+    <sortCondition ref="G2:G41"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2732ED99-57D6-4370-AF6B-2CE20936AA60}" name="#" dataDxfId="19"/>
@@ -2624,8 +2651,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CEB5CD01-35D6-46F3-9680-A4BDE5760A93}" name="Table4" displayName="Table4" ref="A1:H38" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H38" xr:uid="{CEB5CD01-35D6-46F3-9680-A4BDE5760A93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CEB5CD01-35D6-46F3-9680-A4BDE5760A93}" name="Table4" displayName="Table4" ref="A1:H39" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H39" xr:uid="{CEB5CD01-35D6-46F3-9680-A4BDE5760A93}"/>
   <tableColumns count="8">
     <tableColumn id="4" xr3:uid="{A2B1F7F3-5385-4E79-B06A-C5F7E3ACDB1E}" name="EPIC Ref" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{24B7848D-7F8C-4306-8E81-8D1E3DB9E6AE}" name="Feature Ref2" dataDxfId="6"/>
@@ -2939,7 +2966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1021F6-1F59-4996-9A86-B709421DB13F}">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3086,7 +3113,7 @@
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="60" t="s">
         <v>94</v>
       </c>
       <c r="C10" s="4"/>
@@ -3095,7 +3122,7 @@
       <c r="F10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="60" t="s">
         <v>95</v>
       </c>
       <c r="H10" s="4"/>
@@ -3104,7 +3131,7 @@
       <c r="K10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="64" t="s">
+      <c r="L10" s="60" t="s">
         <v>96</v>
       </c>
       <c r="M10" s="4"/>
@@ -3113,7 +3140,7 @@
       <c r="P10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Q10" s="64" t="s">
+      <c r="Q10" s="60" t="s">
         <v>97</v>
       </c>
       <c r="R10" s="4"/>
@@ -3122,153 +3149,153 @@
       <c r="U10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="V10" s="64" t="s">
+      <c r="V10" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="65"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="4"/>
       <c r="D11" s="15"/>
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="67"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="4"/>
       <c r="I11" s="15"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="65"/>
+      <c r="L11" s="61"/>
       <c r="M11" s="4"/>
       <c r="N11" s="15"/>
       <c r="O11" s="4"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="65"/>
+      <c r="Q11" s="61"/>
       <c r="R11" s="4"/>
       <c r="S11" s="15"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-      <c r="V11" s="65"/>
+      <c r="V11" s="61"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
-      <c r="B12" s="65"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="4"/>
       <c r="D12" s="15"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="67"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="4"/>
       <c r="I12" s="15"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="65"/>
+      <c r="L12" s="61"/>
       <c r="M12" s="4"/>
       <c r="N12" s="15"/>
       <c r="O12" s="4"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="65"/>
+      <c r="Q12" s="61"/>
       <c r="R12" s="4"/>
       <c r="S12" s="15"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
-      <c r="V12" s="65"/>
+      <c r="V12" s="61"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="65"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="4"/>
       <c r="D13" s="15"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="67"/>
+      <c r="G13" s="62"/>
       <c r="H13" s="4"/>
       <c r="I13" s="15"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="65"/>
+      <c r="L13" s="61"/>
       <c r="M13" s="4"/>
       <c r="N13" s="15"/>
       <c r="O13" s="4"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="65"/>
+      <c r="Q13" s="61"/>
       <c r="R13" s="4"/>
       <c r="S13" s="15"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
-      <c r="V13" s="65"/>
+      <c r="V13" s="61"/>
     </row>
     <row r="14" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
-      <c r="B14" s="65"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="4"/>
       <c r="D14" s="15"/>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="67"/>
+      <c r="G14" s="62"/>
       <c r="H14" s="4"/>
       <c r="I14" s="15"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="65"/>
+      <c r="L14" s="61"/>
       <c r="M14" s="4"/>
       <c r="N14" s="15"/>
       <c r="O14" s="4"/>
       <c r="P14" s="6"/>
-      <c r="Q14" s="65"/>
+      <c r="Q14" s="61"/>
       <c r="R14" s="4"/>
       <c r="S14" s="15"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
-      <c r="V14" s="65"/>
+      <c r="V14" s="61"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
-      <c r="B15" s="65"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="4"/>
       <c r="D15" s="15"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="67"/>
+      <c r="G15" s="62"/>
       <c r="H15" s="4"/>
       <c r="I15" s="15"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="65"/>
+      <c r="L15" s="61"/>
       <c r="M15" s="4"/>
       <c r="N15" s="15"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="65"/>
+      <c r="Q15" s="61"/>
       <c r="R15" s="4"/>
       <c r="S15" s="15"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
-      <c r="V15" s="65"/>
+      <c r="V15" s="61"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
-      <c r="B16" s="65"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="4"/>
       <c r="D16" s="15"/>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="67"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="4"/>
       <c r="I16" s="15"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="65"/>
+      <c r="L16" s="61"/>
       <c r="M16" s="4"/>
       <c r="N16" s="15"/>
       <c r="O16" s="4"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="65"/>
+      <c r="Q16" s="61"/>
       <c r="R16" s="4"/>
       <c r="S16" s="15"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-      <c r="V16" s="65"/>
+      <c r="V16" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3288,11 +3315,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3325,7 +3352,7 @@
       <c r="G1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="39"/>
+      <c r="K1" s="29"/>
       <c r="L1" s="37"/>
       <c r="M1" s="27"/>
     </row>
@@ -3342,7 +3369,7 @@
       <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="42"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="28"/>
       <c r="G2" s="26"/>
     </row>
@@ -3359,9 +3386,9 @@
       <c r="D3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="43"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="29"/>
-      <c r="G3" s="41"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -3376,7 +3403,7 @@
       <c r="D4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="42"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="28"/>
       <c r="G4" s="26"/>
     </row>
@@ -3393,7 +3420,7 @@
       <c r="D5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="42"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="28"/>
       <c r="G5" s="26"/>
     </row>
@@ -3410,7 +3437,7 @@
       <c r="D6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="42"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="28"/>
       <c r="G6" s="26"/>
     </row>
@@ -3427,7 +3454,7 @@
       <c r="D7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="28"/>
       <c r="G7" s="26"/>
     </row>
@@ -3444,7 +3471,7 @@
       <c r="D8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="28"/>
       <c r="G8" s="26"/>
     </row>
@@ -3461,7 +3488,7 @@
       <c r="D9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="28"/>
       <c r="G9" s="26"/>
     </row>
@@ -3469,18 +3496,18 @@
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="25" t="s">
         <v>145</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="29"/>
-      <c r="G10" s="41"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="1:13" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
@@ -3489,21 +3516,21 @@
       <c r="B11" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="25" t="s">
         <v>127</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="29"/>
-      <c r="G11" s="41"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:13" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="25" t="s">
         <v>253</v>
       </c>
       <c r="C12" s="25" t="s">
@@ -3512,7 +3539,7 @@
       <c r="D12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="42"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="28"/>
       <c r="G12" s="26"/>
     </row>
@@ -3520,7 +3547,7 @@
       <c r="A13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="25" t="s">
         <v>248</v>
       </c>
       <c r="C13" s="25" t="s">
@@ -3529,7 +3556,7 @@
       <c r="D13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="42"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="28"/>
       <c r="G13" s="26"/>
     </row>
@@ -3537,16 +3564,16 @@
       <c r="A14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="25" t="s">
         <v>141</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="43"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="30"/>
       <c r="G14" s="24"/>
     </row>
@@ -3563,7 +3590,7 @@
       <c r="D15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="30"/>
       <c r="G15" s="24"/>
     </row>
@@ -3580,7 +3607,7 @@
       <c r="D16" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="30"/>
       <c r="G16" s="24"/>
     </row>
@@ -3597,9 +3624,9 @@
       <c r="D17" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="29"/>
-      <c r="G17" s="41"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
@@ -3614,26 +3641,26 @@
       <c r="D18" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="43"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="29"/>
-      <c r="G18" s="41"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="25" t="s">
         <v>278</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="43"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="41"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
@@ -3648,7 +3675,7 @@
       <c r="D20" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="43"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="30"/>
       <c r="G20" s="24"/>
     </row>
@@ -3656,35 +3683,35 @@
       <c r="A21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="25" t="s">
         <v>135</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="43"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="41"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="40" t="s">
-        <v>530</v>
+      <c r="C22" s="25" t="s">
+        <v>529</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="41"/>
+      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
@@ -3699,7 +3726,7 @@
       <c r="D23" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="43"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="30"/>
       <c r="G23" s="24"/>
     </row>
@@ -3716,7 +3743,7 @@
       <c r="D24" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="30"/>
       <c r="G24" s="24"/>
     </row>
@@ -3733,7 +3760,7 @@
       <c r="D25" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="43"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="30"/>
       <c r="G25" s="24"/>
     </row>
@@ -3750,7 +3777,7 @@
       <c r="D26" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="43"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="30"/>
       <c r="G26" s="24"/>
     </row>
@@ -3758,35 +3785,35 @@
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="44" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="41"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="44" t="s">
+      <c r="D28" s="24"/>
+      <c r="E28" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="29"/>
-      <c r="G28" s="41"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
@@ -3799,7 +3826,7 @@
         <v>234</v>
       </c>
       <c r="D29" s="27"/>
-      <c r="E29" s="44" t="s">
+      <c r="E29" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="30"/>
@@ -3816,7 +3843,7 @@
         <v>245</v>
       </c>
       <c r="D30" s="27"/>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="30"/>
@@ -3833,7 +3860,7 @@
         <v>228</v>
       </c>
       <c r="D31" s="27"/>
-      <c r="E31" s="44" t="s">
+      <c r="E31" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="29"/>
@@ -3850,7 +3877,7 @@
         <v>54</v>
       </c>
       <c r="D32" s="27"/>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="30"/>
@@ -3866,91 +3893,88 @@
         <v>34</v>
       </c>
       <c r="D33" s="27"/>
-      <c r="E33" s="44" t="s">
+      <c r="E33" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="29" t="s">
+      <c r="A34" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>538</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>532</v>
+      </c>
+      <c r="D34" s="66"/>
+      <c r="E34" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="41"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="66"/>
     </row>
     <row r="35" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="46"/>
+        <v>139</v>
+      </c>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>285</v>
-      </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="29"/>
+        <v>16</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="43"/>
+        <v>18</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="E38" s="41"/>
       <c r="F38" s="29"/>
       <c r="G38" s="37" t="s">
         <v>9</v>
@@ -3958,16 +3982,15 @@
     </row>
     <row r="39" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="42"/>
+        <v>142</v>
+      </c>
+      <c r="E39" s="40"/>
       <c r="F39" s="29"/>
       <c r="G39" s="37" t="s">
         <v>9</v>
@@ -3975,24 +3998,37 @@
     </row>
     <row r="40" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="D40" s="27"/>
-      <c r="E40" s="43"/>
+      <c r="E40" s="39"/>
       <c r="F40" s="29"/>
       <c r="G40" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+    <row r="41" spans="1:7" s="24" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="37" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="42" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B42" s="25"/>
@@ -4057,6 +4093,10 @@
     <row r="57" spans="2:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
+    </row>
+    <row r="58" spans="2:3" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4076,7 +4116,7 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -4087,7 +4127,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>140</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -4258,7 +4298,7 @@
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="25" t="s">
         <v>137</v>
       </c>
       <c r="C13" s="31">
@@ -4342,7 +4382,7 @@
       <c r="A19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="25" t="s">
         <v>111</v>
       </c>
       <c r="C19" s="31">
@@ -4482,7 +4522,7 @@
       <c r="A29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="25" t="s">
         <v>253</v>
       </c>
       <c r="C29" s="31">
@@ -4496,7 +4536,7 @@
       <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="25" t="s">
         <v>248</v>
       </c>
       <c r="C30" s="31">
@@ -4510,7 +4550,7 @@
       <c r="A31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="25" t="s">
         <v>130</v>
       </c>
       <c r="C31" s="31">
@@ -4524,7 +4564,7 @@
       <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="25" t="s">
         <v>134</v>
       </c>
       <c r="C32" s="31">
@@ -4538,7 +4578,7 @@
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="25" t="s">
         <v>249</v>
       </c>
       <c r="C33" s="31">
@@ -4552,7 +4592,7 @@
       <c r="A34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="25" t="s">
         <v>133</v>
       </c>
       <c r="C34" s="31">
@@ -4580,7 +4620,7 @@
       <c r="A36" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="25" t="s">
         <v>132</v>
       </c>
       <c r="C36" s="31">
@@ -4594,7 +4634,7 @@
       <c r="A37" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="25" t="s">
         <v>138</v>
       </c>
       <c r="C37" s="31">
@@ -4636,7 +4676,7 @@
       <c r="A40" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="25" t="s">
         <v>136</v>
       </c>
       <c r="C40" s="31">
@@ -4841,11 +4881,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4862,37 +4902,37 @@
     <col min="11" max="16384" width="8.81640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="57" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:8" s="54" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
         <v>342</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="51" t="s">
         <v>298</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="52" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="166.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="47" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="25" t="s">
@@ -4911,14 +4951,14 @@
         <v>189</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>517</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="78.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="47" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="25" t="s">
@@ -4937,14 +4977,14 @@
         <v>192</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="47" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -4967,10 +5007,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="88.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="47" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="25" t="s">
@@ -4993,10 +5033,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="88.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="47" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -5019,10 +5059,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="94.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="47" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="25" t="s">
@@ -5045,10 +5085,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="94.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="47" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="25" t="s">
@@ -5071,10 +5111,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="178.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="47" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="25" t="s">
@@ -5097,16 +5137,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="25" t="s">
         <v>216</v>
       </c>
       <c r="E10" s="25" t="s">
@@ -5115,18 +5155,18 @@
       <c r="F10" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="25" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -5149,10 +5189,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="25" t="s">
@@ -5175,10 +5215,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="131.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="47" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="25" t="s">
@@ -5201,25 +5241,25 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="148.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="25" t="s">
         <v>285</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="25" t="s">
         <v>284</v>
       </c>
       <c r="H14" s="35" t="s">
@@ -5227,16 +5267,16 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="123.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="47" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="25" t="s">
         <v>127</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -5253,13 +5293,13 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="25" t="s">
         <v>253</v>
       </c>
       <c r="D16" s="25" t="s">
@@ -5279,13 +5319,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="25" t="s">
         <v>248</v>
       </c>
       <c r="D17" s="25" t="s">
@@ -5305,16 +5345,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="25" t="s">
         <v>141</v>
       </c>
       <c r="E18" s="25" t="s">
@@ -5327,18 +5367,18 @@
         <v>288</v>
       </c>
       <c r="H18" s="35" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="137.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="48" t="s">
+        <v>339</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="137.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="51" t="s">
-        <v>339</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>519</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>220</v>
@@ -5357,14 +5397,14 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="149.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="47" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>221</v>
@@ -5383,36 +5423,36 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="25" t="s">
         <v>270</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="G21" s="40" t="s">
+      <c r="G21" s="25" t="s">
         <v>272</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H21" s="25" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="160.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="47" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="25" t="s">
@@ -5431,14 +5471,14 @@
         <v>242</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="191.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="47" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="25" t="s">
@@ -5457,14 +5497,14 @@
         <v>243</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="215" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="47" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -5483,40 +5523,40 @@
         <v>239</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="189" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="25" t="s">
         <v>278</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="25" t="s">
         <v>280</v>
       </c>
-      <c r="G25" s="40" t="s">
+      <c r="G25" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="H25" s="40" t="s">
-        <v>527</v>
+      <c r="H25" s="25" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="182.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="47" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="25" t="s">
@@ -5539,10 +5579,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="44" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -5565,16 +5605,16 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="110" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="25" t="s">
         <v>135</v>
       </c>
       <c r="E28" s="25" t="s">
@@ -5591,51 +5631,51 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="147.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="25" t="s">
         <v>269</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="G29" s="40" t="s">
+      <c r="G29" s="25" t="s">
         <v>274</v>
       </c>
-      <c r="H29" s="40" t="s">
+      <c r="H29" s="25" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="25" t="s">
         <v>142</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="25" t="s">
         <v>294</v>
       </c>
       <c r="H30" s="35" t="s">
@@ -5643,17 +5683,17 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="131" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="40" t="s">
-        <v>530</v>
+      <c r="D31" s="25" t="s">
+        <v>529</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>327</v>
@@ -5669,10 +5709,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="156.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="47" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="25" t="s">
@@ -5688,17 +5728,17 @@
         <v>244</v>
       </c>
       <c r="G32" s="35" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H32" s="35" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="47" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="25" t="s">
@@ -5721,10 +5761,10 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="147" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="45" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="25" t="s">
@@ -5747,10 +5787,10 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="47" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="25" t="s">
@@ -5766,17 +5806,17 @@
         <v>76</v>
       </c>
       <c r="G35" s="35" t="s">
+        <v>527</v>
+      </c>
+      <c r="H35" s="35" t="s">
         <v>528</v>
       </c>
-      <c r="H35" s="35" t="s">
-        <v>529</v>
-      </c>
     </row>
     <row r="36" spans="1:8" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="47" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="25" t="s">
@@ -5799,10 +5839,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -5825,10 +5865,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="46" t="s">
         <v>184</v>
       </c>
       <c r="C38" s="25" t="s">
@@ -5847,7 +5887,33 @@
         <v>187</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>523</v>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="132.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="48" t="s">
+        <v>340</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>530</v>
+      </c>
+      <c r="C39" s="63" t="s">
+        <v>533</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>532</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>531</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>534</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="H39" s="35" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -5865,1439 +5931,1439 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C42F44-6B37-4599-B7B6-D0B0F21F9CB2}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D25" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="60"/>
-    <col min="2" max="3" width="19.54296875" style="60" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" style="60" customWidth="1"/>
-    <col min="6" max="6" width="33.81640625" style="60" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" style="60" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="59" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="60" customWidth="1"/>
-    <col min="10" max="12" width="16.36328125" style="60" customWidth="1"/>
-    <col min="13" max="13" width="27.1796875" style="60" customWidth="1"/>
-    <col min="14" max="14" width="18" style="62" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="60"/>
+    <col min="1" max="1" width="8.7265625" style="57"/>
+    <col min="2" max="3" width="19.54296875" style="57" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="57" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" style="57" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" style="57" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" style="56" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="57" customWidth="1"/>
+    <col min="10" max="12" width="16.36328125" style="57" customWidth="1"/>
+    <col min="13" max="13" width="27.1796875" style="57" customWidth="1"/>
+    <col min="14" max="14" width="18" style="58" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="57"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="57" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="57" t="s">
         <v>344</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="57" t="s">
         <v>420</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="57" t="s">
         <v>382</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="56" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="57" t="s">
         <v>356</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="57" t="s">
         <v>516</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="57" t="s">
         <v>358</v>
       </c>
-      <c r="N1" s="62" t="s">
+      <c r="N1" s="58" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="60">
+      <c r="A2" s="57">
         <v>1</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C2" t="s">
         <v>421</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="57" t="s">
         <v>372</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="57" t="s">
         <v>381</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="57" t="s">
         <v>380</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H2" s="59">
+      <c r="H2" s="56">
         <v>6.5</v>
       </c>
-      <c r="I2" s="60">
+      <c r="I2" s="57">
         <v>1</v>
       </c>
-      <c r="J2" s="60">
+      <c r="J2" s="57">
         <v>9</v>
       </c>
-      <c r="K2" s="60">
+      <c r="K2" s="57">
         <v>4</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N2" s="62">
+      <c r="N2" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="60">
+      <c r="A3" s="57">
         <v>2</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C3" t="s">
         <v>453</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="57" t="s">
         <v>393</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="57" t="s">
         <v>384</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H3" s="59">
+      <c r="H3" s="56">
         <v>6.5</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="57">
         <v>1</v>
       </c>
-      <c r="J3" s="60">
+      <c r="J3" s="57">
         <v>8</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="57">
         <v>3</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N3" s="62">
+      <c r="N3" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="60">
+      <c r="A4" s="57">
         <v>3</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C4" t="s">
         <v>454</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="57" t="s">
         <v>390</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>385</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H4" s="59">
+      <c r="H4" s="56">
         <v>6.5</v>
       </c>
-      <c r="I4" s="60">
+      <c r="I4" s="57">
         <v>1</v>
       </c>
-      <c r="J4" s="60">
+      <c r="J4" s="57">
         <v>7</v>
       </c>
-      <c r="K4" s="60">
+      <c r="K4" s="57">
         <v>5</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="M4" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N4" s="62">
+      <c r="N4" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="60">
+      <c r="A5" s="57">
         <v>4</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C5" t="s">
         <v>457</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="57" t="s">
         <v>395</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="57" t="s">
         <v>386</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="56">
         <v>6.5</v>
       </c>
-      <c r="I5" s="60">
+      <c r="I5" s="57">
         <v>1</v>
       </c>
-      <c r="J5" s="60">
+      <c r="J5" s="57">
         <v>10</v>
       </c>
-      <c r="K5" s="60">
+      <c r="K5" s="57">
         <v>3</v>
       </c>
-      <c r="M5" s="60" t="s">
+      <c r="M5" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N5" s="62">
+      <c r="N5" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="60">
+      <c r="A6" s="57">
         <v>5</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C6" t="s">
         <v>458</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="57" t="s">
         <v>392</v>
       </c>
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="57" t="s">
         <v>387</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H6" s="59">
+      <c r="H6" s="56">
         <v>6.5</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="57">
         <v>1</v>
       </c>
-      <c r="J6" s="60">
+      <c r="J6" s="57">
         <v>4</v>
       </c>
-      <c r="K6" s="60">
+      <c r="K6" s="57">
         <v>2</v>
       </c>
-      <c r="M6" s="60" t="s">
+      <c r="M6" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N6" s="62">
+      <c r="N6" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="60">
+      <c r="A7" s="57">
         <v>6</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C7" t="s">
         <v>455</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="57" t="s">
         <v>391</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="57" t="s">
         <v>388</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="56">
         <v>8</v>
       </c>
-      <c r="I7" s="60">
+      <c r="I7" s="57">
         <v>1</v>
       </c>
-      <c r="J7" s="60">
+      <c r="J7" s="57">
         <v>8</v>
       </c>
-      <c r="K7" s="60">
+      <c r="K7" s="57">
         <v>4</v>
       </c>
-      <c r="M7" s="60" t="s">
+      <c r="M7" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N7" s="62">
+      <c r="N7" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="60">
+      <c r="A8" s="57">
         <v>7</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C8" t="s">
         <v>456</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="57" t="s">
         <v>389</v>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="G8" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H8" s="59">
+      <c r="H8" s="56">
         <v>8.5</v>
       </c>
-      <c r="I8" s="60">
+      <c r="I8" s="57">
         <v>1</v>
       </c>
-      <c r="J8" s="60">
+      <c r="J8" s="57">
         <v>8</v>
       </c>
-      <c r="K8" s="60">
+      <c r="K8" s="57">
         <v>5</v>
       </c>
-      <c r="M8" s="60" t="s">
+      <c r="M8" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="N8" s="62">
+      <c r="N8" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="60">
+      <c r="A9" s="57">
         <v>8</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C9" t="s">
         <v>461</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="57" t="s">
         <v>372</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="57" t="s">
         <v>381</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="57" t="s">
         <v>380</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H9" s="59">
+      <c r="H9" s="56">
         <v>5.5</v>
       </c>
-      <c r="I9" s="60">
+      <c r="I9" s="57">
         <v>2</v>
       </c>
-      <c r="J9" s="60">
+      <c r="J9" s="57">
         <v>9</v>
       </c>
-      <c r="K9" s="60">
+      <c r="K9" s="57">
         <v>4</v>
       </c>
-      <c r="M9" s="60" t="s">
+      <c r="M9" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N9" s="62">
+      <c r="N9" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="60">
+      <c r="A10" s="57">
         <v>9</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C10" t="s">
         <v>462</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="57" t="s">
         <v>393</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="57" t="s">
         <v>384</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H10" s="59">
+      <c r="H10" s="56">
         <v>5.5</v>
       </c>
-      <c r="I10" s="60">
+      <c r="I10" s="57">
         <v>2</v>
       </c>
-      <c r="J10" s="60">
+      <c r="J10" s="57">
         <v>8</v>
       </c>
-      <c r="K10" s="60">
+      <c r="K10" s="57">
         <v>3</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N10" s="62">
+      <c r="N10" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="60">
+      <c r="A11" s="57">
         <v>10</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C11" t="s">
         <v>459</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="57" t="s">
         <v>390</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="57" t="s">
         <v>385</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H11" s="59">
+      <c r="H11" s="56">
         <v>5.5</v>
       </c>
-      <c r="I11" s="60">
+      <c r="I11" s="57">
         <v>2</v>
       </c>
-      <c r="J11" s="60">
+      <c r="J11" s="57">
         <v>7</v>
       </c>
-      <c r="K11" s="60">
+      <c r="K11" s="57">
         <v>5</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="M11" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N11" s="62">
+      <c r="N11" s="58">
         <v>44800</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="60">
+      <c r="A12" s="57">
         <v>11</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C12" t="s">
         <v>460</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="57" t="s">
         <v>395</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="57" t="s">
         <v>386</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G12" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H12" s="59">
+      <c r="H12" s="56">
         <v>5.5</v>
       </c>
-      <c r="I12" s="60">
+      <c r="I12" s="57">
         <v>2</v>
       </c>
-      <c r="J12" s="60">
+      <c r="J12" s="57">
         <v>10</v>
       </c>
-      <c r="K12" s="60">
+      <c r="K12" s="57">
         <v>3</v>
       </c>
-      <c r="M12" s="60" t="s">
+      <c r="M12" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N12" s="62">
+      <c r="N12" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="60">
+      <c r="A13" s="57">
         <v>12</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C13" t="s">
         <v>463</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="E13" s="60" t="s">
+      <c r="E13" s="57" t="s">
         <v>392</v>
       </c>
-      <c r="F13" s="60" t="s">
+      <c r="F13" s="57" t="s">
         <v>387</v>
       </c>
-      <c r="G13" s="60" t="s">
+      <c r="G13" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H13" s="59">
+      <c r="H13" s="56">
         <v>5.5</v>
       </c>
-      <c r="I13" s="60">
+      <c r="I13" s="57">
         <v>2</v>
       </c>
-      <c r="J13" s="60">
+      <c r="J13" s="57">
         <v>4</v>
       </c>
-      <c r="K13" s="60">
+      <c r="K13" s="57">
         <v>2</v>
       </c>
-      <c r="M13" s="60" t="s">
+      <c r="M13" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N13" s="62">
+      <c r="N13" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="60">
+      <c r="A14" s="57">
         <v>13</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C14" t="s">
         <v>464</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="57" t="s">
         <v>391</v>
       </c>
-      <c r="F14" s="60" t="s">
+      <c r="F14" s="57" t="s">
         <v>388</v>
       </c>
-      <c r="G14" s="60" t="s">
+      <c r="G14" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H14" s="59">
+      <c r="H14" s="56">
         <v>7</v>
       </c>
-      <c r="I14" s="60">
+      <c r="I14" s="57">
         <v>2</v>
       </c>
-      <c r="J14" s="60">
+      <c r="J14" s="57">
         <v>8</v>
       </c>
-      <c r="K14" s="60">
+      <c r="K14" s="57">
         <v>4</v>
       </c>
-      <c r="M14" s="60" t="s">
+      <c r="M14" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N14" s="62">
+      <c r="N14" s="58">
         <v>44800</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="60">
+      <c r="A15" s="57">
         <v>14</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C15" t="s">
         <v>465</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="57" t="s">
         <v>389</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H15" s="59">
+      <c r="H15" s="56">
         <v>7.5</v>
       </c>
-      <c r="I15" s="60">
+      <c r="I15" s="57">
         <v>2</v>
       </c>
-      <c r="J15" s="60">
+      <c r="J15" s="57">
         <v>8</v>
       </c>
-      <c r="K15" s="60">
+      <c r="K15" s="57">
         <v>5</v>
       </c>
-      <c r="M15" s="60" t="s">
+      <c r="M15" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="N15" s="62">
+      <c r="N15" s="58">
         <v>44800</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="60">
+      <c r="A16" s="57">
         <v>15</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C16" t="s">
         <v>466</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="57" t="s">
         <v>399</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F16" s="57" t="s">
         <v>398</v>
       </c>
-      <c r="G16" s="60" t="s">
+      <c r="G16" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H16" s="59">
+      <c r="H16" s="56">
         <v>14</v>
       </c>
-      <c r="I16" s="60">
+      <c r="I16" s="57">
         <v>3</v>
       </c>
-      <c r="K16" s="60">
+      <c r="K16" s="57">
         <v>2</v>
       </c>
-      <c r="M16" s="60" t="s">
+      <c r="M16" s="57" t="s">
         <v>503</v>
       </c>
-      <c r="N16" s="62">
+      <c r="N16" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="60">
+      <c r="A17" s="57">
         <v>16</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C17" t="s">
         <v>467</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="57" t="s">
         <v>396</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="57" t="s">
         <v>402</v>
       </c>
-      <c r="G17" s="60" t="s">
+      <c r="G17" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H17" s="59">
+      <c r="H17" s="56">
         <v>18</v>
       </c>
-      <c r="I17" s="60">
+      <c r="I17" s="57">
         <v>3</v>
       </c>
-      <c r="K17" s="60">
+      <c r="K17" s="57">
         <v>4</v>
       </c>
-      <c r="M17" s="60" t="s">
+      <c r="M17" s="57" t="s">
         <v>500</v>
       </c>
-      <c r="N17" s="62">
+      <c r="N17" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="60">
+      <c r="A18" s="57">
         <v>17</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C18" t="s">
         <v>468</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="57" t="s">
         <v>397</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="57" t="s">
         <v>406</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="57" t="s">
         <v>400</v>
       </c>
-      <c r="G18" s="60" t="s">
+      <c r="G18" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H18" s="59">
+      <c r="H18" s="56">
         <v>24</v>
       </c>
-      <c r="I18" s="60">
+      <c r="I18" s="57">
         <v>3</v>
       </c>
-      <c r="K18" s="60">
+      <c r="K18" s="57">
         <v>3</v>
       </c>
-      <c r="M18" s="60" t="s">
+      <c r="M18" s="57" t="s">
         <v>501</v>
       </c>
-      <c r="N18" s="62">
+      <c r="N18" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="60">
+      <c r="A19" s="57">
         <v>18</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C19" t="s">
         <v>469</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H19" s="59">
+      <c r="H19" s="56">
         <v>30</v>
       </c>
-      <c r="I19" s="60">
+      <c r="I19" s="57">
         <v>3</v>
       </c>
-      <c r="K19" s="60">
+      <c r="K19" s="57">
         <v>5</v>
       </c>
-      <c r="M19" s="60" t="s">
+      <c r="M19" s="57" t="s">
         <v>502</v>
       </c>
-      <c r="N19" s="62">
+      <c r="N19" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="60">
+      <c r="A20" s="57">
         <v>19</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C20" t="s">
         <v>470</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="57" t="s">
         <v>408</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H20" s="59">
+      <c r="H20" s="56">
         <v>26.9</v>
       </c>
-      <c r="I20" s="60">
+      <c r="I20" s="57">
         <v>4</v>
       </c>
-      <c r="K20" s="60">
+      <c r="K20" s="57">
         <v>4</v>
       </c>
-      <c r="M20" s="60" t="s">
+      <c r="M20" s="57" t="s">
         <v>511</v>
       </c>
-      <c r="N20" s="62">
+      <c r="N20" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="60">
+      <c r="A21" s="57">
         <v>20</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C21" t="s">
         <v>471</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="57" t="s">
         <v>410</v>
       </c>
-      <c r="E21" s="60" t="s">
+      <c r="E21" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="57" t="s">
         <v>414</v>
       </c>
-      <c r="G21" s="60" t="s">
+      <c r="G21" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H21" s="59">
+      <c r="H21" s="56">
         <v>32.5</v>
       </c>
-      <c r="I21" s="60">
+      <c r="I21" s="57">
         <v>4</v>
       </c>
-      <c r="K21" s="60">
+      <c r="K21" s="57">
         <v>3</v>
       </c>
-      <c r="M21" s="60" t="s">
+      <c r="M21" s="57" t="s">
         <v>512</v>
       </c>
-      <c r="N21" s="62">
+      <c r="N21" s="58">
         <v>44796</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="60">
+      <c r="A22" s="57">
         <v>21</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C22" t="s">
         <v>472</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="57" t="s">
         <v>412</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="57" t="s">
         <v>504</v>
       </c>
-      <c r="G22" s="60" t="s">
+      <c r="G22" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H22" s="59">
+      <c r="H22" s="56">
         <v>36.99</v>
       </c>
-      <c r="I22" s="60">
+      <c r="I22" s="57">
         <v>4</v>
       </c>
-      <c r="K22" s="60">
+      <c r="K22" s="57">
         <v>5</v>
       </c>
-      <c r="M22" s="60" t="s">
+      <c r="M22" s="57" t="s">
         <v>513</v>
       </c>
-      <c r="N22" s="62">
+      <c r="N22" s="58">
         <v>44800</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="60">
+      <c r="A23" s="57">
         <v>22</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C23" t="s">
         <v>473</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="57" t="s">
         <v>416</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="57" t="s">
         <v>417</v>
       </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="57" t="s">
         <v>415</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H23" s="59">
+      <c r="H23" s="56">
         <v>32.5</v>
       </c>
-      <c r="I23" s="60">
+      <c r="I23" s="57">
         <v>4</v>
       </c>
-      <c r="K23" s="60">
+      <c r="K23" s="57">
         <v>4</v>
       </c>
-      <c r="M23" s="60" t="s">
+      <c r="M23" s="57" t="s">
         <v>514</v>
       </c>
-      <c r="N23" s="62">
+      <c r="N23" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="60">
+      <c r="A24" s="57">
         <v>23</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C24" t="s">
         <v>474</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="57" t="s">
         <v>418</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="57" t="s">
         <v>419</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="57" t="s">
         <v>505</v>
       </c>
-      <c r="G24" s="60" t="s">
+      <c r="G24" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H24" s="59">
+      <c r="H24" s="56">
         <v>39.5</v>
       </c>
-      <c r="I24" s="60">
+      <c r="I24" s="57">
         <v>4</v>
       </c>
-      <c r="K24" s="60">
+      <c r="K24" s="57">
         <v>3</v>
       </c>
-      <c r="M24" s="60" t="s">
+      <c r="M24" s="57" t="s">
         <v>515</v>
       </c>
-      <c r="N24" s="62">
+      <c r="N24" s="58">
         <v>44800</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="60">
+      <c r="A25" s="57">
         <v>24</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C25" t="s">
         <v>475</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="57" t="s">
         <v>426</v>
       </c>
-      <c r="F25" s="60" t="s">
+      <c r="F25" s="57" t="s">
         <v>427</v>
       </c>
-      <c r="G25" s="60" t="s">
+      <c r="G25" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H25" s="59">
+      <c r="H25" s="56">
         <v>3.99</v>
       </c>
-      <c r="I25" s="60">
+      <c r="I25" s="57">
         <v>5</v>
       </c>
-      <c r="K25" s="60">
+      <c r="K25" s="57">
         <v>2</v>
       </c>
-      <c r="M25" s="60" t="s">
+      <c r="M25" s="57" t="s">
         <v>428</v>
       </c>
-      <c r="N25" s="62">
+      <c r="N25" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="60">
+      <c r="A26" s="57">
         <v>25</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C26" t="s">
         <v>476</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="57" t="s">
         <v>506</v>
       </c>
-      <c r="E26" s="60" t="s">
+      <c r="E26" s="57" t="s">
         <v>434</v>
       </c>
-      <c r="F26" s="61" t="s">
+      <c r="F26" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="G26" s="60" t="s">
+      <c r="G26" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H26" s="59">
+      <c r="H26" s="56">
         <v>4.99</v>
       </c>
-      <c r="I26" s="60">
+      <c r="I26" s="57">
         <v>5</v>
       </c>
-      <c r="K26" s="60">
+      <c r="K26" s="57">
         <v>3</v>
       </c>
-      <c r="M26" s="60" t="s">
+      <c r="M26" s="57" t="s">
         <v>436</v>
       </c>
-      <c r="N26" s="62">
+      <c r="N26" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="60">
+      <c r="A27" s="57">
         <v>26</v>
       </c>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C27" t="s">
         <v>477</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="57" t="s">
         <v>424</v>
       </c>
-      <c r="E27" s="60" t="s">
+      <c r="E27" s="57" t="s">
         <v>432</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="57" t="s">
         <v>431</v>
       </c>
-      <c r="G27" s="60" t="s">
+      <c r="G27" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H27" s="59">
+      <c r="H27" s="56">
         <v>7.99</v>
       </c>
-      <c r="I27" s="60">
+      <c r="I27" s="57">
         <v>5</v>
       </c>
-      <c r="K27" s="60">
+      <c r="K27" s="57">
         <v>3</v>
       </c>
-      <c r="M27" s="60" t="s">
+      <c r="M27" s="57" t="s">
         <v>430</v>
       </c>
-      <c r="N27" s="62">
+      <c r="N27" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="60">
+      <c r="A28" s="57">
         <v>27</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C28" t="s">
         <v>478</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="57" t="s">
         <v>425</v>
       </c>
-      <c r="E28" s="60" t="s">
+      <c r="E28" s="57" t="s">
         <v>433</v>
       </c>
-      <c r="F28" s="60" t="s">
+      <c r="F28" s="57" t="s">
         <v>507</v>
       </c>
-      <c r="G28" s="60" t="s">
+      <c r="G28" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H28" s="59">
+      <c r="H28" s="56">
         <v>4.99</v>
       </c>
-      <c r="I28" s="60">
+      <c r="I28" s="57">
         <v>5</v>
       </c>
-      <c r="K28" s="60">
+      <c r="K28" s="57">
         <v>4</v>
       </c>
-      <c r="M28" s="60" t="s">
+      <c r="M28" s="57" t="s">
         <v>429</v>
       </c>
-      <c r="N28" s="62">
+      <c r="N28" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="60">
+      <c r="A29" s="57">
         <v>28</v>
       </c>
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C29" t="s">
         <v>479</v>
       </c>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="57" t="s">
         <v>438</v>
       </c>
-      <c r="E29" s="60" t="s">
+      <c r="E29" s="57" t="s">
         <v>440</v>
       </c>
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="57" t="s">
         <v>439</v>
       </c>
-      <c r="G29" s="60" t="s">
+      <c r="G29" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H29" s="59">
+      <c r="H29" s="56">
         <v>2.99</v>
       </c>
-      <c r="I29" s="60">
+      <c r="I29" s="57">
         <v>5</v>
       </c>
-      <c r="K29" s="60">
+      <c r="K29" s="57">
         <v>2</v>
       </c>
-      <c r="M29" s="60" t="s">
+      <c r="M29" s="57" t="s">
         <v>437</v>
       </c>
-      <c r="N29" s="62">
+      <c r="N29" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="60">
+      <c r="A30" s="57">
         <v>29</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C30" t="s">
         <v>480</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="57" t="s">
         <v>442</v>
       </c>
-      <c r="E30" s="60" t="s">
+      <c r="E30" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="F30" s="60" t="s">
+      <c r="F30" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="G30" s="60" t="s">
+      <c r="G30" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H30" s="59">
+      <c r="H30" s="56">
         <v>449</v>
       </c>
-      <c r="I30" s="60">
+      <c r="I30" s="57">
         <v>6</v>
       </c>
-      <c r="K30" s="60">
+      <c r="K30" s="57">
         <v>3</v>
       </c>
-      <c r="M30" s="60" t="s">
+      <c r="M30" s="57" t="s">
         <v>441</v>
       </c>
-      <c r="N30" s="62">
+      <c r="N30" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="60">
+      <c r="A31" s="57">
         <v>30</v>
       </c>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C31" t="s">
         <v>481</v>
       </c>
-      <c r="D31" s="60" t="s">
+      <c r="D31" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="57" t="s">
         <v>448</v>
       </c>
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="57" t="s">
         <v>447</v>
       </c>
-      <c r="G31" s="60" t="s">
+      <c r="G31" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H31" s="59">
+      <c r="H31" s="56">
         <v>429</v>
       </c>
-      <c r="I31" s="60">
+      <c r="I31" s="57">
         <v>6</v>
       </c>
-      <c r="K31" s="60">
+      <c r="K31" s="57">
         <v>3</v>
       </c>
-      <c r="M31" s="60" t="s">
+      <c r="M31" s="57" t="s">
         <v>445</v>
       </c>
-      <c r="N31" s="62">
+      <c r="N31" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="60">
+      <c r="A32" s="57">
         <v>31</v>
       </c>
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C32" t="s">
         <v>482</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="57" t="s">
         <v>449</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="57" t="s">
         <v>450</v>
       </c>
-      <c r="F32" s="60" t="s">
+      <c r="F32" s="57" t="s">
         <v>451</v>
       </c>
-      <c r="G32" s="60" t="s">
+      <c r="G32" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H32" s="59">
+      <c r="H32" s="56">
         <v>775</v>
       </c>
-      <c r="I32" s="60">
+      <c r="I32" s="57">
         <v>6</v>
       </c>
-      <c r="K32" s="60">
+      <c r="K32" s="57">
         <v>5</v>
       </c>
-      <c r="M32" s="60" t="s">
+      <c r="M32" s="57" t="s">
         <v>452</v>
       </c>
-      <c r="N32" s="62">
+      <c r="N32" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="60">
+      <c r="A33" s="57">
         <v>32</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C33" t="s">
         <v>486</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="57" t="s">
         <v>508</v>
       </c>
-      <c r="E33" s="60" t="s">
+      <c r="E33" s="57" t="s">
         <v>485</v>
       </c>
-      <c r="F33" s="60" t="s">
+      <c r="F33" s="57" t="s">
         <v>484</v>
       </c>
-      <c r="G33" s="60" t="s">
+      <c r="G33" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="H33" s="59">
+      <c r="H33" s="56">
         <v>36.99</v>
       </c>
-      <c r="I33" s="60">
+      <c r="I33" s="57">
         <v>6</v>
       </c>
-      <c r="K33" s="60">
+      <c r="K33" s="57">
         <v>4</v>
       </c>
-      <c r="M33" s="60" t="s">
+      <c r="M33" s="57" t="s">
         <v>483</v>
       </c>
-      <c r="N33" s="62">
+      <c r="N33" s="58">
         <v>44799</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="60">
+      <c r="A34" s="57">
         <v>33</v>
       </c>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C34" t="s">
         <v>495</v>
       </c>
-      <c r="D34" s="60" t="s">
+      <c r="D34" s="57" t="s">
         <v>487</v>
       </c>
-      <c r="E34" s="60" t="s">
+      <c r="E34" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="F34" s="60" t="s">
+      <c r="F34" s="57" t="s">
         <v>489</v>
       </c>
-      <c r="G34" s="60" t="s">
+      <c r="G34" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H34" s="59">
+      <c r="H34" s="56">
         <v>24.6</v>
       </c>
-      <c r="I34" s="60">
+      <c r="I34" s="57">
         <v>7</v>
       </c>
-      <c r="K34" s="60">
+      <c r="K34" s="57">
         <v>5</v>
       </c>
-      <c r="M34" s="60" t="s">
+      <c r="M34" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="N34" s="62">
+      <c r="N34" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="60">
+      <c r="A35" s="57">
         <v>34</v>
       </c>
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C35" t="s">
         <v>496</v>
       </c>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="57" t="s">
         <v>490</v>
       </c>
-      <c r="E35" s="60" t="s">
+      <c r="E35" s="57" t="s">
         <v>499</v>
       </c>
-      <c r="F35" s="60" t="s">
+      <c r="F35" s="57" t="s">
         <v>509</v>
       </c>
-      <c r="G35" s="60" t="s">
+      <c r="G35" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H35" s="59">
+      <c r="H35" s="56">
         <v>15</v>
       </c>
-      <c r="I35" s="60">
+      <c r="I35" s="57">
         <v>7</v>
       </c>
-      <c r="K35" s="60">
+      <c r="K35" s="57">
         <v>4</v>
       </c>
-      <c r="M35" s="60" t="s">
+      <c r="M35" s="57" t="s">
         <v>494</v>
       </c>
-      <c r="N35" s="62">
+      <c r="N35" s="58">
         <v>44798</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="60">
+      <c r="A36" s="57">
         <v>35</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C36" t="s">
         <v>497</v>
       </c>
-      <c r="D36" s="60" t="s">
+      <c r="D36" s="57" t="s">
         <v>491</v>
       </c>
-      <c r="E36" s="60" t="s">
+      <c r="E36" s="57" t="s">
         <v>498</v>
       </c>
-      <c r="F36" s="60" t="s">
+      <c r="F36" s="57" t="s">
         <v>510</v>
       </c>
-      <c r="G36" s="60" t="s">
+      <c r="G36" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="H36" s="59">
+      <c r="H36" s="56">
         <v>15</v>
       </c>
-      <c r="I36" s="60">
+      <c r="I36" s="57">
         <v>7</v>
       </c>
-      <c r="K36" s="60">
+      <c r="K36" s="57">
         <v>3</v>
       </c>
-      <c r="M36" s="60" t="s">
+      <c r="M36" s="57" t="s">
         <v>493</v>
       </c>
-      <c r="N36" s="62">
+      <c r="N36" s="58">
         <v>44798</v>
       </c>
     </row>
@@ -7324,128 +7390,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="55" t="s">
         <v>344</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="55" t="s">
         <v>353</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="55" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="58">
+      <c r="A2" s="55">
         <v>1</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="55" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="58">
+      <c r="A3" s="55">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="55" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="58">
+      <c r="A4" s="55">
         <v>3</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="55" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="55" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="58">
+      <c r="A5" s="55">
         <v>4</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="55" t="s">
         <v>362</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="55" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="58">
+      <c r="A6" s="55">
         <v>5</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="55" t="s">
         <v>348</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="55" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="58">
+      <c r="A7" s="55">
         <v>6</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="55" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="55" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="58">
+      <c r="A8" s="55">
         <v>7</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="55" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="58">
+      <c r="A9" s="55">
         <v>8</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="55" t="s">
         <v>355</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="55" t="s">
         <v>367</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="55" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7468,10 +7534,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="63">
+      <c r="A1" s="59">
         <v>44809</v>
       </c>
-      <c r="B1" s="63">
+      <c r="B1" s="59">
         <v>44812</v>
       </c>
     </row>

</xml_diff>